<commit_message>
Timesheet and Workers commit
</commit_message>
<xml_diff>
--- a/src/main/resources/Excel/LoginCredentials.xlsx
+++ b/src/main/resources/Excel/LoginCredentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nisha James\eclipse-workspace\PayrollApplication\src\main\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703662C8-BA83-471B-829C-4B4D88701535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FB5464-03C9-443D-80DA-FD33D2A4CB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{87059EFC-8A0C-455B-AD26-5118BA57C32F}"/>
   </bookViews>
@@ -45,7 +45,7 @@
     <t>carol</t>
   </si>
   <si>
-    <t>1q2w3e4</t>
+    <t>1q2w3e4r</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>